<commit_message>
Summary by Country and Scope
</commit_message>
<xml_diff>
--- a/data/medios_origen.xlsx
+++ b/data/medios_origen.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddeburgos-my.sharepoint.com/personal/vahedo_ubu_es/Documents/Goonies/Tesis Silvita/google-news-french-way-cyl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1700" documentId="8_{7346C9C1-3AAC-4DAF-9414-12FC8F6551AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF7A858B-77EC-4D61-84DB-558E1841CB4B}"/>
+  <xr:revisionPtr revIDLastSave="1710" documentId="8_{7346C9C1-3AAC-4DAF-9414-12FC8F6551AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB9112F0-2EB1-4762-9204-C5F6EE212B92}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="180" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$715</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$716</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2485" uniqueCount="882">
   <si>
     <t>source</t>
   </si>
@@ -3062,8 +3062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D716"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A589" workbookViewId="0">
+      <selection activeCell="D516" sqref="D516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6374,6 +6374,9 @@
         <v>880</v>
       </c>
       <c r="C270" t="s">
+        <v>5</v>
+      </c>
+      <c r="D270" t="s">
         <v>22</v>
       </c>
     </row>
@@ -9482,7 +9485,7 @@
         <v>587</v>
       </c>
       <c r="B522" t="s">
-        <v>588</v>
+        <v>880</v>
       </c>
       <c r="C522" t="s">
         <v>5</v>
@@ -11959,7 +11962,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D715" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:D716" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D716">
       <sortCondition ref="A1:A715"/>
     </sortState>

</xml_diff>